<commit_message>
Data processing and sub-categorization
Co-Authored-By: urvins03 <61550538+urvins03@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/Updated Data/gas_type_form.xlsx
+++ b/Updated Data/gas_type_form.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="11">
   <si>
     <t>Form</t>
   </si>
@@ -25,10 +25,16 @@
     <t>Type</t>
   </si>
   <si>
+    <t>Acetylene</t>
+  </si>
+  <si>
     <t>Hydrogen</t>
   </si>
   <si>
     <t>Other (Specify)</t>
+  </si>
+  <si>
+    <t>Not Labelled</t>
   </si>
   <si>
     <t>Jet from a pressurized source</t>
@@ -398,7 +404,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D8"/>
+  <dimension ref="A1:D10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -423,55 +429,57 @@
         <v>3</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C2">
+        <v>1</v>
+      </c>
+      <c r="D2">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3">
         <v>9</v>
       </c>
-      <c r="D2">
+      <c r="D3">
         <v>1.7</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4">
-      <c r="A3" s="1"/>
-      <c r="B3" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C3">
-        <v>4</v>
-      </c>
-      <c r="D3">
-        <v>0.8</v>
       </c>
     </row>
     <row r="4" spans="1:4">
       <c r="A4" s="1"/>
       <c r="B4" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4">
         <v>4</v>
       </c>
-      <c r="C4">
-        <v>3</v>
-      </c>
       <c r="D4">
-        <v>0.6</v>
+        <v>0.8</v>
       </c>
     </row>
     <row r="5" spans="1:4">
       <c r="A5" s="1"/>
       <c r="B5" s="1" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C5">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D5">
-        <v>0.4</v>
+        <v>0.6</v>
       </c>
     </row>
     <row r="6" spans="1:4">
       <c r="A6" s="1"/>
       <c r="B6" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C6">
         <v>2</v>
@@ -481,11 +489,9 @@
       </c>
     </row>
     <row r="7" spans="1:4">
-      <c r="A7" s="1" t="s">
-        <v>4</v>
-      </c>
+      <c r="A7" s="1"/>
       <c r="B7" s="1" t="s">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="C7">
         <v>2</v>
@@ -506,10 +512,36 @@
         <v>0.2</v>
       </c>
     </row>
+    <row r="9" spans="1:4">
+      <c r="A9" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C9">
+        <v>2</v>
+      </c>
+      <c r="D9">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4">
+      <c r="A10" s="1"/>
+      <c r="B10" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C10">
+        <v>1</v>
+      </c>
+      <c r="D10">
+        <v>0.2</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="2">
-    <mergeCell ref="A2:A6"/>
-    <mergeCell ref="A7:A8"/>
+    <mergeCell ref="A3:A8"/>
+    <mergeCell ref="A9:A10"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>